<commit_message>
Feat: Approach 2 for entity recognition implemented
</commit_message>
<xml_diff>
--- a/data/root_word_corpus.xlsx
+++ b/data/root_word_corpus.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$65</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t xml:space="preserve">zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taluka</t>
   </si>
   <si>
     <t xml:space="preserve">invoice</t>
@@ -256,6 +262,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -345,13 +352,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -551,7 +558,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,10 +566,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,10 +577,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,7 +591,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,10 +599,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,10 +610,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,7 +624,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +632,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,7 +646,7 @@
         <v>32</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,10 +654,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +668,7 @@
         <v>34</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,10 +676,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,10 +687,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,10 +698,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,7 +712,7 @@
         <v>37</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,10 +720,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,10 +731,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,7 +745,7 @@
         <v>41</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,10 +753,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,10 +764,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,10 +775,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,7 +789,7 @@
         <v>44</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,7 +800,7 @@
         <v>45</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,10 +819,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,10 +830,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,7 +844,7 @@
         <v>50</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,10 +852,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,10 +863,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,10 +874,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,7 +888,7 @@
         <v>53</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +899,7 @@
         <v>54</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,10 +907,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,10 +918,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,10 +929,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,10 +940,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +954,7 @@
         <v>59</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,7 +965,7 @@
         <v>60</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,7 +976,7 @@
         <v>61</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +987,7 @@
         <v>62</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +998,7 @@
         <v>63</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,7 +1009,7 @@
         <v>64</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1020,7 @@
         <v>65</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,10 +1028,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,10 +1039,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,10 +1050,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,10 +1061,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,14 +1075,36 @@
         <v>72</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D65"/>
+  <autoFilter ref="A1:D67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Update: Added sales root words
</commit_message>
<xml_diff>
--- a/data/root_word_corpus.xlsx
+++ b/data/root_word_corpus.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$70</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="77">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">disburse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loan</t>
   </si>
   <si>
     <t xml:space="preserve">company</t>
@@ -352,13 +358,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -646,7 +652,7 @@
         <v>32</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,10 +660,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +674,7 @@
         <v>34</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,10 +682,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,7 +696,7 @@
         <v>36</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,10 +704,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,10 +715,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,10 +726,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,7 +740,7 @@
         <v>39</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,10 +748,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,10 +759,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +773,7 @@
         <v>43</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,10 +781,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,10 +792,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,10 +803,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,7 +817,7 @@
         <v>46</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,7 +828,7 @@
         <v>47</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,7 +839,7 @@
         <v>48</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,10 +847,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,10 +858,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +872,7 @@
         <v>52</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,10 +880,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,10 +891,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,10 +902,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +916,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,7 +927,7 @@
         <v>56</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,10 +935,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,10 +946,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,10 +957,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,7 +971,7 @@
         <v>60</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,10 +979,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,10 +990,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,10 +1001,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,10 +1012,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,10 +1023,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,10 +1034,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,10 +1045,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,10 +1056,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,10 +1067,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,10 +1078,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,10 +1089,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,14 +1100,47 @@
         <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>71</v>
+      <c r="D68" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D67"/>
+  <autoFilter ref="A1:D70"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Update: Added val, vol entity mappings
</commit_message>
<xml_diff>
--- a/data/root_word_corpus.xlsx
+++ b/data/root_word_corpus.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$70</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$72</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t xml:space="preserve">inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val</t>
   </si>
   <si>
     <t xml:space="preserve">quantity</t>
@@ -358,13 +364,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -946,7 +952,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>51</v>
@@ -957,10 +963,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,10 +974,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,10 +985,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,10 +996,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,10 +1007,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1021,7 @@
         <v>63</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,7 +1032,7 @@
         <v>64</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,7 +1043,7 @@
         <v>65</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1054,7 @@
         <v>66</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1059,7 +1065,7 @@
         <v>67</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1076,7 @@
         <v>68</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1087,7 @@
         <v>69</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,10 +1095,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,10 +1106,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D67" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,10 +1117,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,10 +1128,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,14 +1142,36 @@
         <v>76</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D70"/>
+  <autoFilter ref="A1:D72"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
FEAT: First cut results published
</commit_message>
<xml_diff>
--- a/data/root_word_corpus.xlsx
+++ b/data/root_word_corpus.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$72</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -181,6 +181,9 @@
     <t xml:space="preserve">Sales</t>
   </si>
   <si>
+    <t xml:space="preserve">sales</t>
+  </si>
+  <si>
     <t xml:space="preserve">sold</t>
   </si>
   <si>
@@ -203,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disbursed</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
@@ -364,13 +370,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+      <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -908,7 +914,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>51</v>
@@ -919,7 +925,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>51</v>
@@ -974,7 +980,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>51</v>
@@ -985,10 +991,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,10 +1002,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,10 +1013,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,10 +1024,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,10 +1035,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,7 +1049,7 @@
         <v>65</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,7 +1060,7 @@
         <v>66</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,7 +1071,7 @@
         <v>67</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1082,7 @@
         <v>68</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,7 +1093,7 @@
         <v>69</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,7 +1104,7 @@
         <v>70</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,7 +1115,7 @@
         <v>71</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,10 +1123,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,10 +1134,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D69" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,10 +1145,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,10 +1156,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,11 +1170,33 @@
         <v>78</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D72"/>
+  <autoFilter ref="A1:D74"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>